<commit_message>
updated gpt experiments to the latest version
</commit_message>
<xml_diff>
--- a/03_Classifier/app_src/gpt_models_experiments/GPT_MODELS_RESULTS.xlsx
+++ b/03_Classifier/app_src/gpt_models_experiments/GPT_MODELS_RESULTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scoala\RESEARCH\MLCP\03_Classifier\app_src\gpt_models_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3073F906-CFEB-4C7B-AE97-C14305F67AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B9613-F7B8-4C42-A70E-37D7CC581368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27135" yWindow="3030" windowWidth="18045" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="2460" windowWidth="33495" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>gpt4o</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>top 20 outside dataset</t>
+  </si>
+  <si>
+    <t>o3-mini</t>
+  </si>
+  <si>
+    <t>10.35% yes</t>
+  </si>
+  <si>
+    <t>5.77% yes</t>
   </si>
 </sst>
 </file>
@@ -99,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E20"/>
+  <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,155 +467,152 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>154</v>
+      </c>
+      <c r="D6">
+        <v>0.59</v>
+      </c>
+      <c r="E6">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>0.46</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>0.68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>0.45</v>
-      </c>
-      <c r="E7">
-        <v>0.66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>0.45</v>
+      </c>
+      <c r="E8">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>90</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>0.49</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>0.69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>21</v>
-      </c>
-      <c r="D9">
-        <v>0.42</v>
-      </c>
-      <c r="E9">
-        <v>0.64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>150</v>
+      </c>
+      <c r="D10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E10">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0.42</v>
+      </c>
+      <c r="E11">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>18</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>0.39</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>0.61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>118</v>
-      </c>
-      <c r="D11">
-        <v>0.46</v>
-      </c>
-      <c r="E11">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>16</v>
-      </c>
-      <c r="D12">
-        <v>0.44</v>
-      </c>
-      <c r="E12">
-        <v>0.74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="D13">
-        <v>0.35</v>
+        <v>0.46</v>
       </c>
       <c r="E13">
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="D14">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
       <c r="E14">
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="E15">
-        <v>0.68</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,72 +620,165 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="E16">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="D17">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="E17">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>143</v>
+      </c>
+      <c r="D18">
+        <v>0.53</v>
+      </c>
+      <c r="E18">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
         <v>0</v>
       </c>
-      <c r="C18">
-        <v>16</v>
-      </c>
-      <c r="D18">
-        <v>0.42</v>
-      </c>
-      <c r="E18">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
       <c r="C19">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D19">
-        <v>0.34</v>
+        <v>0.41</v>
       </c>
       <c r="E19">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>0.36</v>
+      </c>
+      <c r="E20">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C21">
+        <v>122</v>
+      </c>
+      <c r="D21">
+        <v>0.44</v>
+      </c>
+      <c r="E21">
+        <v>0.68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>178</v>
+      </c>
+      <c r="D22">
+        <v>0.48</v>
+      </c>
+      <c r="E22">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>0.42</v>
+      </c>
+      <c r="E23">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>0.34</v>
+      </c>
+      <c r="E24">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
         <v>90</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>0.44</v>
       </c>
-      <c r="E20">
+      <c r="E25">
         <v>0.72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>140</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+      <c r="E26">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>